<commit_message>
Fix template formatting priority
</commit_message>
<xml_diff>
--- a/examsLinks.xlsx
+++ b/examsLinks.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="51180" yWindow="12780" windowWidth="25760" windowHeight="16660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="51200" yWindow="12780" windowWidth="25760" windowHeight="16660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -217,22 +217,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" shrinkToFit="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1" readingOrder="2"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" shrinkToFit="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" shrinkToFit="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -243,6 +231,18 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -255,67 +255,12 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="0"/>
   </cellStyles>
-  <dxfs count="168">
+  <dxfs count="25">
     <dxf>
       <fill>
         <patternFill>
           <bgColor theme="7" tint="0.7999816888943144"/>
         </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray0625">
-          <fgColor auto="1"/>
-          <bgColor theme="6" tint="0.3999450666829432"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray0625">
-          <bgColor theme="6" tint="0.3999450666829432"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.7999816888943144"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray0625"/>
       </fill>
     </dxf>
     <dxf>
@@ -376,36 +321,68 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <condense val="0"/>
-        <color theme="1"/>
-        <extend val="0"/>
-        <sz val="14"/>
-        <vertAlign val="baseline"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.7999816888943144"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <condense val="0"/>
-        <color theme="1"/>
-        <extend val="0"/>
-        <sz val="14"/>
-        <vertAlign val="baseline"/>
-        <scheme val="minor"/>
+        <color rgb="FF9C0006"/>
       </font>
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="gray0625">
+          <fgColor auto="1"/>
+          <bgColor theme="6" tint="0.3999450666829432"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="gray0625">
+          <bgColor theme="6" tint="0.3999450666829432"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="gray0625">
+          <bgColor theme="2" tint="-0.249946592608417"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.7999816888943144"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -521,1095 +498,35 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <condense val="0"/>
+        <color theme="1"/>
+        <extend val="0"/>
+        <sz val="14"/>
+        <vertAlign val="baseline"/>
+        <scheme val="minor"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <condense val="0"/>
+        <color theme="1"/>
+        <extend val="0"/>
+        <sz val="14"/>
+        <vertAlign val="baseline"/>
+        <scheme val="minor"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray0625">
-          <bgColor theme="6" tint="0.3999450666829432"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray0625">
-          <fgColor auto="1"/>
-          <bgColor theme="6" tint="0.3999450666829432"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.7999816888943144"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray0625"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.7999816888943144"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray0625"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray0625">
-          <fgColor auto="1"/>
-          <bgColor theme="6" tint="0.3999450666829432"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray0625">
-          <bgColor theme="6" tint="0.3999450666829432"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.7999816888943144"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray0625"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray0625">
-          <fgColor auto="1"/>
-          <bgColor theme="6" tint="0.3999450666829432"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray0625">
-          <bgColor theme="6" tint="0.3999450666829432"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.7999816888943144"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray0625"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray0625">
-          <fgColor auto="1"/>
-          <bgColor theme="6" tint="0.3999450666829432"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray0625">
-          <bgColor theme="6" tint="0.3999450666829432"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.7999816888943144"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray0625"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray0625">
-          <fgColor auto="1"/>
-          <bgColor theme="6" tint="0.3999450666829432"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray0625">
-          <bgColor theme="6" tint="0.3999450666829432"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.7999816888943144"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray0625"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray0625">
-          <fgColor auto="1"/>
-          <bgColor theme="6" tint="0.3999450666829432"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray0625">
-          <bgColor theme="6" tint="0.3999450666829432"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.7999816888943144"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf/>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray0625">
-          <fgColor auto="1"/>
-          <bgColor theme="6" tint="0.3999450666829432"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray0625">
-          <bgColor theme="6" tint="0.3999450666829432"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.7999816888943144"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf/>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray0625">
-          <fgColor auto="1"/>
-          <bgColor theme="6" tint="0.3999450666829432"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray0625">
-          <bgColor theme="6" tint="0.3999450666829432"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.7999816888943144"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf/>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray0625">
-          <fgColor auto="1"/>
-          <bgColor theme="6" tint="0.3999450666829432"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray0625">
-          <bgColor theme="6" tint="0.3999450666829432"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.7999816888943144"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf/>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray0625">
-          <fgColor auto="1"/>
-          <bgColor theme="6" tint="0.3999450666829432"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray0625">
-          <bgColor theme="6" tint="0.3999450666829432"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.7999816888943144"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf/>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray0625">
-          <fgColor auto="1"/>
-          <bgColor theme="6" tint="0.3999450666829432"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray0625">
-          <bgColor theme="6" tint="0.3999450666829432"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.7999816888943144"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf/>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray0625">
-          <fgColor auto="1"/>
-          <bgColor theme="6" tint="0.3999450666829432"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray0625">
-          <bgColor theme="6" tint="0.3999450666829432"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf/>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.7999816888943144"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf/>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray0625">
-          <fgColor auto="1"/>
-          <bgColor theme="6" tint="0.3999450666829432"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray0625">
-          <bgColor theme="6" tint="0.3999450666829432"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf/>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.7999816888943144"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf/>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray0625">
-          <fgColor auto="1"/>
-          <bgColor theme="6" tint="0.3999450666829432"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray0625">
-          <bgColor theme="6" tint="0.3999450666829432"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf/>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.7999816888943144"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf/>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray0625">
-          <fgColor auto="1"/>
-          <bgColor theme="6" tint="0.3999450666829432"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray0625">
-          <bgColor theme="6" tint="0.3999450666829432"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.7999816888943144"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray0625">
-          <fgColor auto="1"/>
-          <bgColor theme="6" tint="0.3999450666829432"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray0625">
-          <bgColor theme="6" tint="0.3999450666829432"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.7999816888943144"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray0625">
-          <fgColor auto="1"/>
-          <bgColor theme="6" tint="0.3999450666829432"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray0625">
-          <bgColor theme="6" tint="0.3999450666829432"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.7999816888943144"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray0625">
-          <fgColor auto="1"/>
-          <bgColor theme="6" tint="0.3999450666829432"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray0625">
-          <bgColor theme="6" tint="0.3999450666829432"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.7999816888943144"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray0625">
-          <fgColor auto="1"/>
-          <bgColor theme="6" tint="0.3999450666829432"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray0625">
-          <bgColor theme="6" tint="0.3999450666829432"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.7999816888943144"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray0625">
-          <fgColor auto="1"/>
-          <bgColor theme="6" tint="0.3999450666829432"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray0625">
-          <bgColor theme="6" tint="0.3999450666829432"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.7999816888943144"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray0625">
-          <fgColor auto="1"/>
-          <bgColor theme="6" tint="0.3999450666829432"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray0625">
-          <bgColor theme="6" tint="0.3999450666829432"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1685,16 +602,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A15:G95" headerRowCount="1" totalsRowShown="0" headerRowDxfId="15" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A15:G95" headerRowCount="1" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
   <autoFilter ref="A15:G95"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="שנה" dataDxfId="23"/>
-    <tableColumn id="2" name="סמסטר" dataDxfId="22"/>
-    <tableColumn id="3" name="מועד" dataDxfId="21"/>
-    <tableColumn id="4" name="לינק" dataDxfId="20"/>
-    <tableColumn id="5" name="בוצע?" dataDxfId="19"/>
-    <tableColumn id="6" name="פתרון" dataDxfId="18"/>
-    <tableColumn id="7" name="הערות" dataDxfId="17"/>
+    <tableColumn id="1" name="שנה" dataDxfId="22"/>
+    <tableColumn id="2" name="סמסטר" dataDxfId="21"/>
+    <tableColumn id="3" name="מועד" dataDxfId="20"/>
+    <tableColumn id="4" name="לינק" dataDxfId="19"/>
+    <tableColumn id="5" name="בוצע?" dataDxfId="18"/>
+    <tableColumn id="6" name="פתרון" dataDxfId="17"/>
+    <tableColumn id="7" name="הערות" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2003,15 +920,15 @@
   </sheetPr>
   <dimension ref="A1:I95"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A4" zoomScale="168" zoomScaleNormal="188" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView rightToLeft="1" tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
   <cols>
-    <col width="10.33203125" customWidth="1" style="14" min="1" max="1"/>
-    <col width="13.33203125" bestFit="1" customWidth="1" style="14" min="2" max="2"/>
-    <col width="10.83203125" customWidth="1" style="14" min="3" max="6"/>
+    <col width="10.33203125" customWidth="1" style="10" min="1" max="1"/>
+    <col width="13.33203125" bestFit="1" customWidth="1" style="10" min="2" max="2"/>
+    <col width="10.83203125" customWidth="1" style="10" min="3" max="6"/>
     <col width="45.1640625" customWidth="1" style="3" min="7" max="7"/>
     <col width="7.83203125" bestFit="1" customWidth="1" style="3" min="8" max="8"/>
     <col width="10.83203125" customWidth="1" style="3" min="9" max="16384"/>
@@ -2019,7 +936,7 @@
   <sheetData>
     <row r="1"/>
     <row r="2">
-      <c r="A2" s="9" t="inlineStr">
+      <c r="A2" s="13" t="inlineStr">
         <is>
           <t>מרקרים אוטומטיים</t>
         </is>
@@ -2028,12 +945,12 @@
       <c r="C2" s="17" t="n"/>
     </row>
     <row r="3" ht="34" customHeight="1">
-      <c r="A3" s="9" t="inlineStr">
+      <c r="A3" s="13" t="inlineStr">
         <is>
           <t>מרקר\דוגמה</t>
         </is>
       </c>
-      <c r="B3" s="9" t="inlineStr">
+      <c r="B3" s="13" t="inlineStr">
         <is>
           <t>תיאור</t>
         </is>
@@ -2046,7 +963,7 @@
           <t>חסר</t>
         </is>
       </c>
-      <c r="B4" s="10" t="inlineStr">
+      <c r="B4" s="12" t="inlineStr">
         <is>
           <t>אין לינק</t>
         </is>
@@ -2068,7 +985,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="B6" s="10" t="inlineStr">
+      <c r="B6" s="12" t="inlineStr">
         <is>
           <t>בתהליך</t>
         </is>
@@ -2081,7 +998,7 @@
           <t>v</t>
         </is>
       </c>
-      <c r="B7" s="10" t="inlineStr">
+      <c r="B7" s="12" t="inlineStr">
         <is>
           <t>בוצע</t>
         </is>
@@ -2094,7 +1011,7 @@
           <t>x</t>
         </is>
       </c>
-      <c r="B8" s="10" t="inlineStr">
+      <c r="B8" s="12" t="inlineStr">
         <is>
           <t>לא יבוצע</t>
         </is>
@@ -2102,41 +1019,41 @@
       <c r="C8" s="17" t="n"/>
     </row>
     <row r="9">
-      <c r="A9" s="15" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="B9" s="10" t="inlineStr">
+      <c r="A9" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="B9" s="12" t="inlineStr">
         <is>
           <t>אין מבחן/פתרון</t>
         </is>
       </c>
       <c r="C9" s="17" t="n"/>
-      <c r="E9" s="14" t="inlineStr">
+      <c r="E9" s="10" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="10">
+      <c r="A10" s="12">
         <f>YEAR(TODAY())-10</f>
         <v/>
       </c>
-      <c r="B10" s="10" t="inlineStr">
+      <c r="B10" s="12" t="inlineStr">
         <is>
           <t>ישן מ10 שנים</t>
         </is>
       </c>
-      <c r="C10" s="10" t="n"/>
+      <c r="C10" s="17" t="n"/>
     </row>
     <row r="11">
-      <c r="A11" s="10">
+      <c r="A11" s="12">
         <f>YEAR(TODAY())-5</f>
         <v/>
       </c>
-      <c r="B11" s="10" t="inlineStr">
+      <c r="B11" s="12" t="inlineStr">
         <is>
           <t>ישן מ5 שנים</t>
         </is>
@@ -2144,11 +1061,11 @@
       <c r="C11" s="17" t="n"/>
     </row>
     <row r="12">
-      <c r="A12" s="10">
+      <c r="A12" s="12">
         <f>YEAR(TODAY())</f>
         <v/>
       </c>
-      <c r="B12" s="10" t="inlineStr">
+      <c r="B12" s="12" t="inlineStr">
         <is>
           <t>5 שנים אחרונות</t>
         </is>
@@ -2156,60 +1073,60 @@
       <c r="C12" s="17" t="n"/>
     </row>
     <row r="13">
-      <c r="A13" s="13" t="n"/>
-      <c r="B13" s="13" t="n"/>
-      <c r="C13" s="14" t="n"/>
+      <c r="A13" s="9" t="n"/>
+      <c r="B13" s="9" t="n"/>
+      <c r="C13" s="10" t="n"/>
     </row>
     <row r="14">
-      <c r="A14" s="13" t="n"/>
+      <c r="A14" s="9" t="n"/>
     </row>
     <row r="15">
-      <c r="A15" s="14" t="inlineStr">
+      <c r="A15" s="10" t="inlineStr">
         <is>
           <t>שנה</t>
         </is>
       </c>
-      <c r="B15" s="14" t="inlineStr">
+      <c r="B15" s="10" t="inlineStr">
         <is>
           <t>סמסטר</t>
         </is>
       </c>
-      <c r="C15" s="14" t="inlineStr">
+      <c r="C15" s="10" t="inlineStr">
         <is>
           <t>מועד</t>
         </is>
       </c>
-      <c r="D15" s="14" t="inlineStr">
+      <c r="D15" s="10" t="inlineStr">
         <is>
           <t>לינק</t>
         </is>
       </c>
-      <c r="E15" s="14" t="inlineStr">
+      <c r="E15" s="10" t="inlineStr">
         <is>
           <t>בוצע?</t>
         </is>
       </c>
-      <c r="F15" s="14" t="inlineStr">
+      <c r="F15" s="10" t="inlineStr">
         <is>
           <t>פתרון</t>
         </is>
       </c>
-      <c r="G15" s="14" t="inlineStr">
+      <c r="G15" s="10" t="inlineStr">
         <is>
           <t>הערות</t>
         </is>
       </c>
     </row>
     <row r="16" ht="18" customHeight="1">
-      <c r="A16" s="14" t="n">
+      <c r="A16" s="10" t="n">
         <v>2003</v>
       </c>
-      <c r="B16" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C16" s="14" t="inlineStr">
+      <c r="B16" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C16" s="10" t="inlineStr">
         <is>
           <t>א</t>
         </is>
@@ -2224,24 +1141,24 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F16" s="14" t="inlineStr">
+      <c r="F16" s="10" t="inlineStr">
         <is>
           <t>/</t>
         </is>
       </c>
       <c r="G16" s="1" t="n"/>
-      <c r="I16" s="14" t="n"/>
+      <c r="I16" s="10" t="n"/>
     </row>
     <row r="17" ht="18" customHeight="1">
-      <c r="A17" s="14" t="n">
+      <c r="A17" s="10" t="n">
         <v>2003</v>
       </c>
-      <c r="B17" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C17" s="14" t="inlineStr">
+      <c r="B17" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C17" s="10" t="inlineStr">
         <is>
           <t>ב</t>
         </is>
@@ -2256,7 +1173,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F17" s="14" t="inlineStr">
+      <c r="F17" s="10" t="inlineStr">
         <is>
           <t>/</t>
         </is>
@@ -2264,15 +1181,15 @@
       <c r="G17" s="5" t="n"/>
     </row>
     <row r="18" ht="18" customHeight="1">
-      <c r="A18" s="14" t="n">
+      <c r="A18" s="10" t="n">
         <v>2003</v>
       </c>
-      <c r="B18" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C18" s="14" t="inlineStr">
+      <c r="B18" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C18" s="10" t="inlineStr">
         <is>
           <t>א</t>
         </is>
@@ -2287,7 +1204,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F18" s="14" t="inlineStr">
+      <c r="F18" s="10" t="inlineStr">
         <is>
           <t>/</t>
         </is>
@@ -2295,15 +1212,15 @@
       <c r="G18" s="5" t="n"/>
     </row>
     <row r="19" ht="18" customHeight="1">
-      <c r="A19" s="14" t="n">
+      <c r="A19" s="10" t="n">
         <v>2003</v>
       </c>
-      <c r="B19" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C19" s="14" t="inlineStr">
+      <c r="B19" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C19" s="10" t="inlineStr">
         <is>
           <t>ב</t>
         </is>
@@ -2318,7 +1235,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F19" s="14" t="inlineStr">
+      <c r="F19" s="10" t="inlineStr">
         <is>
           <t>/</t>
         </is>
@@ -2326,15 +1243,15 @@
       <c r="G19" s="5" t="n"/>
     </row>
     <row r="20" ht="18" customHeight="1">
-      <c r="A20" s="14" t="n">
+      <c r="A20" s="10" t="n">
         <v>2004</v>
       </c>
-      <c r="B20" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C20" s="14" t="inlineStr">
+      <c r="B20" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C20" s="10" t="inlineStr">
         <is>
           <t>א</t>
         </is>
@@ -2349,7 +1266,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F20" s="14" t="inlineStr">
+      <c r="F20" s="10" t="inlineStr">
         <is>
           <t>/</t>
         </is>
@@ -2357,15 +1274,15 @@
       <c r="G20" s="5" t="n"/>
     </row>
     <row r="21" ht="18" customHeight="1">
-      <c r="A21" s="14" t="n">
+      <c r="A21" s="10" t="n">
         <v>2004</v>
       </c>
-      <c r="B21" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C21" s="14" t="inlineStr">
+      <c r="B21" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C21" s="10" t="inlineStr">
         <is>
           <t>ב</t>
         </is>
@@ -2380,7 +1297,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F21" s="14" t="inlineStr">
+      <c r="F21" s="10" t="inlineStr">
         <is>
           <t>/</t>
         </is>
@@ -2388,15 +1305,15 @@
       <c r="G21" s="5" t="n"/>
     </row>
     <row r="22" ht="18" customHeight="1">
-      <c r="A22" s="14" t="n">
+      <c r="A22" s="10" t="n">
         <v>2004</v>
       </c>
-      <c r="B22" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C22" s="14" t="inlineStr">
+      <c r="B22" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C22" s="10" t="inlineStr">
         <is>
           <t>א</t>
         </is>
@@ -2411,7 +1328,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F22" s="14" t="inlineStr">
+      <c r="F22" s="10" t="inlineStr">
         <is>
           <t>/</t>
         </is>
@@ -2419,15 +1336,15 @@
       <c r="G22" s="5" t="n"/>
     </row>
     <row r="23" ht="18" customHeight="1">
-      <c r="A23" s="14" t="n">
+      <c r="A23" s="10" t="n">
         <v>2004</v>
       </c>
-      <c r="B23" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C23" s="14" t="inlineStr">
+      <c r="B23" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C23" s="10" t="inlineStr">
         <is>
           <t>ב</t>
         </is>
@@ -2442,7 +1359,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F23" s="14" t="inlineStr">
+      <c r="F23" s="10" t="inlineStr">
         <is>
           <t>/</t>
         </is>
@@ -2450,15 +1367,15 @@
       <c r="G23" s="5" t="n"/>
     </row>
     <row r="24" ht="18" customHeight="1">
-      <c r="A24" s="14" t="n">
+      <c r="A24" s="10" t="n">
         <v>2005</v>
       </c>
-      <c r="B24" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C24" s="14" t="inlineStr">
+      <c r="B24" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C24" s="10" t="inlineStr">
         <is>
           <t>א</t>
         </is>
@@ -2473,7 +1390,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F24" s="14" t="inlineStr">
+      <c r="F24" s="10" t="inlineStr">
         <is>
           <t>/</t>
         </is>
@@ -2481,15 +1398,15 @@
       <c r="G24" s="5" t="n"/>
     </row>
     <row r="25" ht="18" customHeight="1">
-      <c r="A25" s="14" t="n">
+      <c r="A25" s="10" t="n">
         <v>2005</v>
       </c>
-      <c r="B25" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C25" s="14" t="inlineStr">
+      <c r="B25" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C25" s="10" t="inlineStr">
         <is>
           <t>ב</t>
         </is>
@@ -2504,7 +1421,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F25" s="14" t="inlineStr">
+      <c r="F25" s="10" t="inlineStr">
         <is>
           <t>/</t>
         </is>
@@ -2512,15 +1429,15 @@
       <c r="G25" s="5" t="n"/>
     </row>
     <row r="26" ht="18" customHeight="1">
-      <c r="A26" s="14" t="n">
+      <c r="A26" s="10" t="n">
         <v>2005</v>
       </c>
-      <c r="B26" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C26" s="14" t="inlineStr">
+      <c r="B26" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C26" s="10" t="inlineStr">
         <is>
           <t>א</t>
         </is>
@@ -2543,15 +1460,15 @@
       <c r="G26" s="5" t="n"/>
     </row>
     <row r="27" ht="18" customHeight="1">
-      <c r="A27" s="14" t="n">
+      <c r="A27" s="10" t="n">
         <v>2005</v>
       </c>
-      <c r="B27" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C27" s="14" t="inlineStr">
+      <c r="B27" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C27" s="10" t="inlineStr">
         <is>
           <t>ב</t>
         </is>
@@ -2574,15 +1491,15 @@
       <c r="G27" s="5" t="n"/>
     </row>
     <row r="28" ht="18" customHeight="1">
-      <c r="A28" s="14" t="n">
+      <c r="A28" s="10" t="n">
         <v>2006</v>
       </c>
-      <c r="B28" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C28" s="14" t="inlineStr">
+      <c r="B28" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C28" s="10" t="inlineStr">
         <is>
           <t>א</t>
         </is>
@@ -2605,15 +1522,15 @@
       <c r="G28" s="5" t="n"/>
     </row>
     <row r="29" ht="18" customHeight="1">
-      <c r="A29" s="14" t="n">
+      <c r="A29" s="10" t="n">
         <v>2006</v>
       </c>
-      <c r="B29" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C29" s="14" t="inlineStr">
+      <c r="B29" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C29" s="10" t="inlineStr">
         <is>
           <t>ב</t>
         </is>
@@ -2636,15 +1553,15 @@
       <c r="G29" s="5" t="n"/>
     </row>
     <row r="30" ht="18" customHeight="1">
-      <c r="A30" s="14" t="n">
+      <c r="A30" s="10" t="n">
         <v>2006</v>
       </c>
-      <c r="B30" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C30" s="14" t="inlineStr">
+      <c r="B30" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C30" s="10" t="inlineStr">
         <is>
           <t>א</t>
         </is>
@@ -2667,15 +1584,15 @@
       <c r="G30" s="5" t="n"/>
     </row>
     <row r="31" ht="18" customHeight="1">
-      <c r="A31" s="14" t="n">
+      <c r="A31" s="10" t="n">
         <v>2006</v>
       </c>
-      <c r="B31" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C31" s="14" t="inlineStr">
+      <c r="B31" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C31" s="10" t="inlineStr">
         <is>
           <t>ב</t>
         </is>
@@ -2698,15 +1615,15 @@
       <c r="G31" s="5" t="n"/>
     </row>
     <row r="32" ht="18" customHeight="1">
-      <c r="A32" s="14" t="n">
+      <c r="A32" s="10" t="n">
         <v>2007</v>
       </c>
-      <c r="B32" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C32" s="14" t="inlineStr">
+      <c r="B32" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C32" s="10" t="inlineStr">
         <is>
           <t>א</t>
         </is>
@@ -2729,15 +1646,15 @@
       <c r="G32" s="5" t="n"/>
     </row>
     <row r="33" ht="18" customHeight="1">
-      <c r="A33" s="14" t="n">
+      <c r="A33" s="10" t="n">
         <v>2007</v>
       </c>
-      <c r="B33" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C33" s="14" t="inlineStr">
+      <c r="B33" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C33" s="10" t="inlineStr">
         <is>
           <t>ב</t>
         </is>
@@ -2760,15 +1677,15 @@
       <c r="G33" s="5" t="n"/>
     </row>
     <row r="34" ht="18" customHeight="1">
-      <c r="A34" s="14" t="n">
+      <c r="A34" s="10" t="n">
         <v>2007</v>
       </c>
-      <c r="B34" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C34" s="14" t="inlineStr">
+      <c r="B34" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C34" s="10" t="inlineStr">
         <is>
           <t>א</t>
         </is>
@@ -2791,15 +1708,15 @@
       <c r="G34" s="5" t="n"/>
     </row>
     <row r="35" ht="18" customHeight="1">
-      <c r="A35" s="14" t="n">
+      <c r="A35" s="10" t="n">
         <v>2007</v>
       </c>
-      <c r="B35" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C35" s="14" t="inlineStr">
+      <c r="B35" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C35" s="10" t="inlineStr">
         <is>
           <t>ב</t>
         </is>
@@ -2822,15 +1739,15 @@
       <c r="G35" s="5" t="n"/>
     </row>
     <row r="36" ht="18" customHeight="1">
-      <c r="A36" s="14" t="n">
+      <c r="A36" s="10" t="n">
         <v>2008</v>
       </c>
-      <c r="B36" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C36" s="14" t="inlineStr">
+      <c r="B36" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C36" s="10" t="inlineStr">
         <is>
           <t>א</t>
         </is>
@@ -2853,15 +1770,15 @@
       <c r="G36" s="5" t="n"/>
     </row>
     <row r="37" ht="18" customHeight="1">
-      <c r="A37" s="14" t="n">
+      <c r="A37" s="10" t="n">
         <v>2008</v>
       </c>
-      <c r="B37" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C37" s="14" t="inlineStr">
+      <c r="B37" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C37" s="10" t="inlineStr">
         <is>
           <t>ב</t>
         </is>
@@ -2884,15 +1801,15 @@
       <c r="G37" s="5" t="n"/>
     </row>
     <row r="38" ht="18" customHeight="1">
-      <c r="A38" s="14" t="n">
+      <c r="A38" s="10" t="n">
         <v>2008</v>
       </c>
-      <c r="B38" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C38" s="14" t="inlineStr">
+      <c r="B38" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C38" s="10" t="inlineStr">
         <is>
           <t>א</t>
         </is>
@@ -2915,15 +1832,15 @@
       <c r="G38" s="5" t="n"/>
     </row>
     <row r="39" ht="18" customHeight="1">
-      <c r="A39" s="14" t="n">
+      <c r="A39" s="10" t="n">
         <v>2008</v>
       </c>
-      <c r="B39" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C39" s="14" t="inlineStr">
+      <c r="B39" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C39" s="10" t="inlineStr">
         <is>
           <t>ב</t>
         </is>
@@ -2946,15 +1863,15 @@
       <c r="G39" s="5" t="n"/>
     </row>
     <row r="40" ht="18" customHeight="1">
-      <c r="A40" s="14" t="n">
+      <c r="A40" s="10" t="n">
         <v>2009</v>
       </c>
-      <c r="B40" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C40" s="14" t="inlineStr">
+      <c r="B40" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C40" s="10" t="inlineStr">
         <is>
           <t>א</t>
         </is>
@@ -2977,15 +1894,15 @@
       <c r="G40" s="5" t="n"/>
     </row>
     <row r="41" ht="18" customHeight="1">
-      <c r="A41" s="14" t="n">
+      <c r="A41" s="10" t="n">
         <v>2009</v>
       </c>
-      <c r="B41" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C41" s="14" t="inlineStr">
+      <c r="B41" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C41" s="10" t="inlineStr">
         <is>
           <t>ב</t>
         </is>
@@ -3008,15 +1925,15 @@
       <c r="G41" s="5" t="n"/>
     </row>
     <row r="42" ht="18" customHeight="1">
-      <c r="A42" s="14" t="n">
+      <c r="A42" s="10" t="n">
         <v>2009</v>
       </c>
-      <c r="B42" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C42" s="14" t="inlineStr">
+      <c r="B42" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C42" s="10" t="inlineStr">
         <is>
           <t>א</t>
         </is>
@@ -3039,15 +1956,15 @@
       <c r="G42" s="5" t="n"/>
     </row>
     <row r="43" ht="18" customHeight="1">
-      <c r="A43" s="14" t="n">
+      <c r="A43" s="10" t="n">
         <v>2009</v>
       </c>
-      <c r="B43" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C43" s="14" t="inlineStr">
+      <c r="B43" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C43" s="10" t="inlineStr">
         <is>
           <t>ב</t>
         </is>
@@ -3070,15 +1987,15 @@
       <c r="G43" s="5" t="n"/>
     </row>
     <row r="44" ht="18" customHeight="1">
-      <c r="A44" s="14" t="n">
+      <c r="A44" s="10" t="n">
         <v>2010</v>
       </c>
-      <c r="B44" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C44" s="14" t="inlineStr">
+      <c r="B44" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C44" s="10" t="inlineStr">
         <is>
           <t>א</t>
         </is>
@@ -3101,15 +2018,15 @@
       <c r="G44" s="5" t="n"/>
     </row>
     <row r="45" ht="18" customHeight="1">
-      <c r="A45" s="14" t="n">
+      <c r="A45" s="10" t="n">
         <v>2010</v>
       </c>
-      <c r="B45" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C45" s="14" t="inlineStr">
+      <c r="B45" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C45" s="10" t="inlineStr">
         <is>
           <t>ב</t>
         </is>
@@ -3132,15 +2049,15 @@
       <c r="G45" s="5" t="n"/>
     </row>
     <row r="46" ht="18" customHeight="1">
-      <c r="A46" s="14" t="n">
+      <c r="A46" s="10" t="n">
         <v>2010</v>
       </c>
-      <c r="B46" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C46" s="14" t="inlineStr">
+      <c r="B46" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C46" s="10" t="inlineStr">
         <is>
           <t>א</t>
         </is>
@@ -3163,15 +2080,15 @@
       <c r="G46" s="5" t="n"/>
     </row>
     <row r="47" ht="18" customHeight="1">
-      <c r="A47" s="14" t="n">
+      <c r="A47" s="10" t="n">
         <v>2010</v>
       </c>
-      <c r="B47" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C47" s="14" t="inlineStr">
+      <c r="B47" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C47" s="10" t="inlineStr">
         <is>
           <t>ב</t>
         </is>
@@ -3194,15 +2111,15 @@
       <c r="G47" s="5" t="n"/>
     </row>
     <row r="48" ht="18" customHeight="1">
-      <c r="A48" s="14" t="n">
+      <c r="A48" s="10" t="n">
         <v>2011</v>
       </c>
-      <c r="B48" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C48" s="14" t="inlineStr">
+      <c r="B48" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C48" s="10" t="inlineStr">
         <is>
           <t>א</t>
         </is>
@@ -3225,15 +2142,15 @@
       <c r="G48" s="5" t="n"/>
     </row>
     <row r="49" ht="18" customHeight="1">
-      <c r="A49" s="14" t="n">
+      <c r="A49" s="10" t="n">
         <v>2011</v>
       </c>
-      <c r="B49" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C49" s="14" t="inlineStr">
+      <c r="B49" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C49" s="10" t="inlineStr">
         <is>
           <t>ב</t>
         </is>
@@ -3256,15 +2173,15 @@
       <c r="G49" s="5" t="n"/>
     </row>
     <row r="50" ht="18" customHeight="1">
-      <c r="A50" s="14" t="n">
+      <c r="A50" s="10" t="n">
         <v>2011</v>
       </c>
-      <c r="B50" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C50" s="14" t="inlineStr">
+      <c r="B50" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C50" s="10" t="inlineStr">
         <is>
           <t>א</t>
         </is>
@@ -3287,15 +2204,15 @@
       <c r="G50" s="5" t="n"/>
     </row>
     <row r="51" ht="18" customHeight="1">
-      <c r="A51" s="14" t="n">
+      <c r="A51" s="10" t="n">
         <v>2011</v>
       </c>
-      <c r="B51" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C51" s="14" t="inlineStr">
+      <c r="B51" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C51" s="10" t="inlineStr">
         <is>
           <t>ב</t>
         </is>
@@ -3318,15 +2235,15 @@
       <c r="G51" s="5" t="n"/>
     </row>
     <row r="52" ht="18" customHeight="1">
-      <c r="A52" s="14" t="n">
+      <c r="A52" s="10" t="n">
         <v>2012</v>
       </c>
-      <c r="B52" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C52" s="14" t="inlineStr">
+      <c r="B52" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C52" s="10" t="inlineStr">
         <is>
           <t>א</t>
         </is>
@@ -3349,15 +2266,15 @@
       <c r="G52" s="5" t="n"/>
     </row>
     <row r="53" ht="18" customHeight="1">
-      <c r="A53" s="14" t="n">
+      <c r="A53" s="10" t="n">
         <v>2012</v>
       </c>
-      <c r="B53" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C53" s="14" t="inlineStr">
+      <c r="B53" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C53" s="10" t="inlineStr">
         <is>
           <t>ב</t>
         </is>
@@ -3380,15 +2297,15 @@
       <c r="G53" s="5" t="n"/>
     </row>
     <row r="54" ht="18" customHeight="1">
-      <c r="A54" s="14" t="n">
+      <c r="A54" s="10" t="n">
         <v>2012</v>
       </c>
-      <c r="B54" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C54" s="14" t="inlineStr">
+      <c r="B54" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C54" s="10" t="inlineStr">
         <is>
           <t>א</t>
         </is>
@@ -3411,15 +2328,15 @@
       <c r="G54" s="5" t="n"/>
     </row>
     <row r="55" ht="18" customHeight="1">
-      <c r="A55" s="14" t="n">
+      <c r="A55" s="10" t="n">
         <v>2012</v>
       </c>
-      <c r="B55" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C55" s="14" t="inlineStr">
+      <c r="B55" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C55" s="10" t="inlineStr">
         <is>
           <t>ב</t>
         </is>
@@ -3442,15 +2359,15 @@
       <c r="G55" s="5" t="n"/>
     </row>
     <row r="56" ht="18" customHeight="1">
-      <c r="A56" s="14" t="n">
+      <c r="A56" s="10" t="n">
         <v>2013</v>
       </c>
-      <c r="B56" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C56" s="14" t="inlineStr">
+      <c r="B56" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C56" s="10" t="inlineStr">
         <is>
           <t>א</t>
         </is>
@@ -3473,15 +2390,15 @@
       <c r="G56" s="5" t="n"/>
     </row>
     <row r="57" ht="18" customHeight="1">
-      <c r="A57" s="14" t="n">
+      <c r="A57" s="10" t="n">
         <v>2013</v>
       </c>
-      <c r="B57" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C57" s="14" t="inlineStr">
+      <c r="B57" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C57" s="10" t="inlineStr">
         <is>
           <t>ב</t>
         </is>
@@ -3504,15 +2421,15 @@
       <c r="G57" s="5" t="n"/>
     </row>
     <row r="58" ht="18" customHeight="1">
-      <c r="A58" s="14" t="n">
+      <c r="A58" s="10" t="n">
         <v>2013</v>
       </c>
-      <c r="B58" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C58" s="14" t="inlineStr">
+      <c r="B58" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C58" s="10" t="inlineStr">
         <is>
           <t>א</t>
         </is>
@@ -3535,15 +2452,15 @@
       <c r="G58" s="5" t="n"/>
     </row>
     <row r="59" ht="18" customHeight="1">
-      <c r="A59" s="14" t="n">
+      <c r="A59" s="10" t="n">
         <v>2013</v>
       </c>
-      <c r="B59" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C59" s="14" t="inlineStr">
+      <c r="B59" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C59" s="10" t="inlineStr">
         <is>
           <t>ב</t>
         </is>
@@ -3566,15 +2483,15 @@
       <c r="G59" s="5" t="n"/>
     </row>
     <row r="60" ht="18" customHeight="1">
-      <c r="A60" s="14" t="n">
+      <c r="A60" s="10" t="n">
         <v>2014</v>
       </c>
-      <c r="B60" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C60" s="14" t="inlineStr">
+      <c r="B60" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C60" s="10" t="inlineStr">
         <is>
           <t>א</t>
         </is>
@@ -3597,15 +2514,15 @@
       <c r="G60" s="5" t="n"/>
     </row>
     <row r="61" ht="18" customHeight="1">
-      <c r="A61" s="14" t="n">
+      <c r="A61" s="10" t="n">
         <v>2014</v>
       </c>
-      <c r="B61" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C61" s="14" t="inlineStr">
+      <c r="B61" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C61" s="10" t="inlineStr">
         <is>
           <t>ב</t>
         </is>
@@ -3628,15 +2545,15 @@
       <c r="G61" s="5" t="n"/>
     </row>
     <row r="62" ht="18" customHeight="1">
-      <c r="A62" s="14" t="n">
+      <c r="A62" s="10" t="n">
         <v>2014</v>
       </c>
-      <c r="B62" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C62" s="14" t="inlineStr">
+      <c r="B62" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C62" s="10" t="inlineStr">
         <is>
           <t>א</t>
         </is>
@@ -3659,15 +2576,15 @@
       <c r="G62" s="5" t="n"/>
     </row>
     <row r="63" ht="18" customHeight="1">
-      <c r="A63" s="14" t="n">
+      <c r="A63" s="10" t="n">
         <v>2014</v>
       </c>
-      <c r="B63" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C63" s="14" t="inlineStr">
+      <c r="B63" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C63" s="10" t="inlineStr">
         <is>
           <t>ב</t>
         </is>
@@ -3690,15 +2607,15 @@
       <c r="G63" s="5" t="n"/>
     </row>
     <row r="64" ht="18" customHeight="1">
-      <c r="A64" s="14" t="n">
+      <c r="A64" s="10" t="n">
         <v>2015</v>
       </c>
-      <c r="B64" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C64" s="14" t="inlineStr">
+      <c r="B64" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C64" s="10" t="inlineStr">
         <is>
           <t>א</t>
         </is>
@@ -3721,15 +2638,15 @@
       <c r="G64" s="5" t="n"/>
     </row>
     <row r="65" ht="18" customHeight="1">
-      <c r="A65" s="14" t="n">
+      <c r="A65" s="10" t="n">
         <v>2015</v>
       </c>
-      <c r="B65" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C65" s="14" t="inlineStr">
+      <c r="B65" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C65" s="10" t="inlineStr">
         <is>
           <t>ב</t>
         </is>
@@ -3752,15 +2669,15 @@
       <c r="G65" s="5" t="n"/>
     </row>
     <row r="66" ht="18" customHeight="1">
-      <c r="A66" s="14" t="n">
+      <c r="A66" s="10" t="n">
         <v>2015</v>
       </c>
-      <c r="B66" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C66" s="14" t="inlineStr">
+      <c r="B66" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C66" s="10" t="inlineStr">
         <is>
           <t>א</t>
         </is>
@@ -3783,15 +2700,15 @@
       <c r="G66" s="5" t="n"/>
     </row>
     <row r="67" ht="18" customHeight="1">
-      <c r="A67" s="14" t="n">
+      <c r="A67" s="10" t="n">
         <v>2015</v>
       </c>
-      <c r="B67" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C67" s="14" t="inlineStr">
+      <c r="B67" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C67" s="10" t="inlineStr">
         <is>
           <t>ב</t>
         </is>
@@ -3814,15 +2731,15 @@
       <c r="G67" s="5" t="n"/>
     </row>
     <row r="68" ht="18" customHeight="1">
-      <c r="A68" s="14" t="n">
+      <c r="A68" s="10" t="n">
         <v>2016</v>
       </c>
-      <c r="B68" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C68" s="14" t="inlineStr">
+      <c r="B68" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C68" s="10" t="inlineStr">
         <is>
           <t>א</t>
         </is>
@@ -3845,15 +2762,15 @@
       <c r="G68" s="5" t="n"/>
     </row>
     <row r="69" ht="18" customHeight="1">
-      <c r="A69" s="14" t="n">
+      <c r="A69" s="10" t="n">
         <v>2016</v>
       </c>
-      <c r="B69" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C69" s="14" t="inlineStr">
+      <c r="B69" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C69" s="10" t="inlineStr">
         <is>
           <t>ב</t>
         </is>
@@ -3876,15 +2793,15 @@
       <c r="G69" s="5" t="n"/>
     </row>
     <row r="70" ht="18" customHeight="1">
-      <c r="A70" s="14" t="n">
+      <c r="A70" s="10" t="n">
         <v>2016</v>
       </c>
-      <c r="B70" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C70" s="14" t="inlineStr">
+      <c r="B70" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C70" s="10" t="inlineStr">
         <is>
           <t>א</t>
         </is>
@@ -3907,25 +2824,25 @@
       <c r="G70" s="5" t="n"/>
     </row>
     <row r="71" ht="18" customHeight="1">
-      <c r="A71" s="14" t="n">
+      <c r="A71" s="10" t="n">
         <v>2016</v>
       </c>
-      <c r="B71" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C71" s="14" t="inlineStr">
-        <is>
-          <t>ב</t>
-        </is>
-      </c>
-      <c r="D71" s="14" t="inlineStr">
+      <c r="B71" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C71" s="10" t="inlineStr">
+        <is>
+          <t>ב</t>
+        </is>
+      </c>
+      <c r="D71" s="10" t="inlineStr">
         <is>
           <t>חסר</t>
         </is>
       </c>
-      <c r="F71" s="14" t="inlineStr">
+      <c r="F71" s="10" t="inlineStr">
         <is>
           <t>/</t>
         </is>
@@ -3933,25 +2850,25 @@
       <c r="G71" s="5" t="n"/>
     </row>
     <row r="72" ht="18" customHeight="1">
-      <c r="A72" s="14" t="n">
+      <c r="A72" s="10" t="n">
         <v>2017</v>
       </c>
-      <c r="B72" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C72" s="14" t="inlineStr">
-        <is>
-          <t>א</t>
-        </is>
-      </c>
-      <c r="D72" s="14" t="inlineStr">
+      <c r="B72" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C72" s="10" t="inlineStr">
+        <is>
+          <t>א</t>
+        </is>
+      </c>
+      <c r="D72" s="10" t="inlineStr">
         <is>
           <t>חסר</t>
         </is>
       </c>
-      <c r="F72" s="14" t="inlineStr">
+      <c r="F72" s="10" t="inlineStr">
         <is>
           <t>/</t>
         </is>
@@ -3959,25 +2876,25 @@
       <c r="G72" s="5" t="n"/>
     </row>
     <row r="73" ht="18" customHeight="1">
-      <c r="A73" s="14" t="n">
+      <c r="A73" s="10" t="n">
         <v>2017</v>
       </c>
-      <c r="B73" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C73" s="14" t="inlineStr">
-        <is>
-          <t>ב</t>
-        </is>
-      </c>
-      <c r="D73" s="14" t="inlineStr">
+      <c r="B73" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C73" s="10" t="inlineStr">
+        <is>
+          <t>ב</t>
+        </is>
+      </c>
+      <c r="D73" s="10" t="inlineStr">
         <is>
           <t>חסר</t>
         </is>
       </c>
-      <c r="F73" s="14" t="inlineStr">
+      <c r="F73" s="10" t="inlineStr">
         <is>
           <t>/</t>
         </is>
@@ -3985,15 +2902,15 @@
       <c r="G73" s="5" t="n"/>
     </row>
     <row r="74" ht="18" customHeight="1">
-      <c r="A74" s="14" t="n">
+      <c r="A74" s="10" t="n">
         <v>2017</v>
       </c>
-      <c r="B74" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C74" s="14" t="inlineStr">
+      <c r="B74" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C74" s="10" t="inlineStr">
         <is>
           <t>א</t>
         </is>
@@ -4016,15 +2933,15 @@
       <c r="G74" s="5" t="n"/>
     </row>
     <row r="75" ht="18" customHeight="1">
-      <c r="A75" s="14" t="n">
+      <c r="A75" s="10" t="n">
         <v>2017</v>
       </c>
-      <c r="B75" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C75" s="14" t="inlineStr">
+      <c r="B75" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C75" s="10" t="inlineStr">
         <is>
           <t>ב</t>
         </is>
@@ -4047,15 +2964,15 @@
       <c r="G75" s="5" t="n"/>
     </row>
     <row r="76" ht="18" customHeight="1">
-      <c r="A76" s="14" t="n">
+      <c r="A76" s="10" t="n">
         <v>2018</v>
       </c>
-      <c r="B76" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C76" s="14" t="inlineStr">
+      <c r="B76" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C76" s="10" t="inlineStr">
         <is>
           <t>א</t>
         </is>
@@ -4078,15 +2995,15 @@
       <c r="G76" s="5" t="n"/>
     </row>
     <row r="77" ht="18" customHeight="1">
-      <c r="A77" s="14" t="n">
+      <c r="A77" s="10" t="n">
         <v>2018</v>
       </c>
-      <c r="B77" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C77" s="14" t="inlineStr">
+      <c r="B77" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C77" s="10" t="inlineStr">
         <is>
           <t>ב</t>
         </is>
@@ -4109,15 +3026,15 @@
       <c r="G77" s="5" t="n"/>
     </row>
     <row r="78" ht="18" customHeight="1">
-      <c r="A78" s="14" t="n">
+      <c r="A78" s="10" t="n">
         <v>2018</v>
       </c>
-      <c r="B78" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C78" s="14" t="inlineStr">
+      <c r="B78" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C78" s="10" t="inlineStr">
         <is>
           <t>א</t>
         </is>
@@ -4140,20 +3057,20 @@
       <c r="G78" s="5" t="n"/>
     </row>
     <row r="79" ht="18" customHeight="1">
-      <c r="A79" s="14" t="n">
+      <c r="A79" s="10" t="n">
         <v>2018</v>
       </c>
-      <c r="B79" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C79" s="14" t="inlineStr">
-        <is>
-          <t>ב</t>
-        </is>
-      </c>
-      <c r="D79" s="14" t="inlineStr">
+      <c r="B79" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C79" s="10" t="inlineStr">
+        <is>
+          <t>ב</t>
+        </is>
+      </c>
+      <c r="D79" s="10" t="inlineStr">
         <is>
           <t>חסר</t>
         </is>
@@ -4171,15 +3088,15 @@
       <c r="G79" s="5" t="n"/>
     </row>
     <row r="80" ht="18" customHeight="1">
-      <c r="A80" s="14" t="n">
+      <c r="A80" s="10" t="n">
         <v>2019</v>
       </c>
-      <c r="B80" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C80" s="14" t="inlineStr">
+      <c r="B80" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C80" s="10" t="inlineStr">
         <is>
           <t>א</t>
         </is>
@@ -4202,15 +3119,15 @@
       <c r="G80" s="5" t="n"/>
     </row>
     <row r="81" ht="18" customHeight="1">
-      <c r="A81" s="14" t="n">
+      <c r="A81" s="10" t="n">
         <v>2019</v>
       </c>
-      <c r="B81" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C81" s="14" t="inlineStr">
+      <c r="B81" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C81" s="10" t="inlineStr">
         <is>
           <t>ב</t>
         </is>
@@ -4233,15 +3150,15 @@
       <c r="G81" s="5" t="n"/>
     </row>
     <row r="82" ht="18" customHeight="1">
-      <c r="A82" s="14" t="n">
+      <c r="A82" s="10" t="n">
         <v>2019</v>
       </c>
-      <c r="B82" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C82" s="14" t="inlineStr">
+      <c r="B82" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C82" s="10" t="inlineStr">
         <is>
           <t>א</t>
         </is>
@@ -4264,15 +3181,15 @@
       <c r="G82" s="5" t="n"/>
     </row>
     <row r="83" ht="18" customHeight="1">
-      <c r="A83" s="14" t="n">
+      <c r="A83" s="10" t="n">
         <v>2019</v>
       </c>
-      <c r="B83" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C83" s="14" t="inlineStr">
+      <c r="B83" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C83" s="10" t="inlineStr">
         <is>
           <t>ב</t>
         </is>
@@ -4295,15 +3212,15 @@
       <c r="G83" s="5" t="n"/>
     </row>
     <row r="84" ht="18" customHeight="1">
-      <c r="A84" s="14" t="n">
+      <c r="A84" s="10" t="n">
         <v>2020</v>
       </c>
-      <c r="B84" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C84" s="14" t="inlineStr">
+      <c r="B84" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C84" s="10" t="inlineStr">
         <is>
           <t>א</t>
         </is>
@@ -4326,15 +3243,15 @@
       <c r="G84" s="5" t="n"/>
     </row>
     <row r="85" ht="18" customHeight="1">
-      <c r="A85" s="14" t="n">
+      <c r="A85" s="10" t="n">
         <v>2020</v>
       </c>
-      <c r="B85" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C85" s="14" t="inlineStr">
+      <c r="B85" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C85" s="10" t="inlineStr">
         <is>
           <t>ב</t>
         </is>
@@ -4357,15 +3274,15 @@
       <c r="G85" s="5" t="n"/>
     </row>
     <row r="86" ht="18" customHeight="1">
-      <c r="A86" s="14" t="n">
+      <c r="A86" s="10" t="n">
         <v>2020</v>
       </c>
-      <c r="B86" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C86" s="14" t="inlineStr">
+      <c r="B86" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C86" s="10" t="inlineStr">
         <is>
           <t>א</t>
         </is>
@@ -4388,15 +3305,15 @@
       <c r="G86" s="5" t="n"/>
     </row>
     <row r="87" ht="18" customHeight="1">
-      <c r="A87" s="14" t="n">
+      <c r="A87" s="10" t="n">
         <v>2020</v>
       </c>
-      <c r="B87" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C87" s="14" t="inlineStr">
+      <c r="B87" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C87" s="10" t="inlineStr">
         <is>
           <t>ב</t>
         </is>
@@ -4419,15 +3336,15 @@
       <c r="G87" s="5" t="n"/>
     </row>
     <row r="88" ht="18" customHeight="1">
-      <c r="A88" s="14" t="n">
+      <c r="A88" s="10" t="n">
         <v>2021</v>
       </c>
-      <c r="B88" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C88" s="14" t="inlineStr">
+      <c r="B88" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C88" s="10" t="inlineStr">
         <is>
           <t>א</t>
         </is>
@@ -4450,15 +3367,15 @@
       <c r="G88" s="5" t="n"/>
     </row>
     <row r="89" ht="18" customHeight="1">
-      <c r="A89" s="14" t="n">
+      <c r="A89" s="10" t="n">
         <v>2021</v>
       </c>
-      <c r="B89" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C89" s="14" t="inlineStr">
+      <c r="B89" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C89" s="10" t="inlineStr">
         <is>
           <t>ב</t>
         </is>
@@ -4473,7 +3390,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F89" s="14" t="inlineStr">
+      <c r="F89" s="10" t="inlineStr">
         <is>
           <t>/</t>
         </is>
@@ -4481,15 +3398,15 @@
       <c r="G89" s="5" t="n"/>
     </row>
     <row r="90" ht="18" customHeight="1">
-      <c r="A90" s="14" t="n">
+      <c r="A90" s="10" t="n">
         <v>2021</v>
       </c>
-      <c r="B90" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C90" s="14" t="inlineStr">
+      <c r="B90" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C90" s="10" t="inlineStr">
         <is>
           <t>א</t>
         </is>
@@ -4504,7 +3421,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F90" s="14" t="inlineStr">
+      <c r="F90" s="10" t="inlineStr">
         <is>
           <t>/</t>
         </is>
@@ -4512,15 +3429,15 @@
       <c r="G90" s="5" t="n"/>
     </row>
     <row r="91" ht="18" customHeight="1">
-      <c r="A91" s="14" t="n">
+      <c r="A91" s="10" t="n">
         <v>2021</v>
       </c>
-      <c r="B91" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C91" s="14" t="inlineStr">
+      <c r="B91" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C91" s="10" t="inlineStr">
         <is>
           <t>ב</t>
         </is>
@@ -4535,7 +3452,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F91" s="14" t="inlineStr">
+      <c r="F91" s="10" t="inlineStr">
         <is>
           <t>/</t>
         </is>
@@ -4543,15 +3460,15 @@
       <c r="G91" s="5" t="n"/>
     </row>
     <row r="92" ht="18" customHeight="1">
-      <c r="A92" s="14" t="n">
+      <c r="A92" s="10" t="n">
         <v>2022</v>
       </c>
-      <c r="B92" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C92" s="14" t="inlineStr">
+      <c r="B92" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C92" s="10" t="inlineStr">
         <is>
           <t>א</t>
         </is>
@@ -4566,7 +3483,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F92" s="14" t="inlineStr">
+      <c r="F92" s="10" t="inlineStr">
         <is>
           <t>/</t>
         </is>
@@ -4574,15 +3491,15 @@
       <c r="G92" s="5" t="n"/>
     </row>
     <row r="93" ht="18" customHeight="1">
-      <c r="A93" s="14" t="n">
+      <c r="A93" s="10" t="n">
         <v>2022</v>
       </c>
-      <c r="B93" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C93" s="14" t="inlineStr">
+      <c r="B93" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C93" s="10" t="inlineStr">
         <is>
           <t>ב</t>
         </is>
@@ -4597,7 +3514,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F93" s="14" t="inlineStr">
+      <c r="F93" s="10" t="inlineStr">
         <is>
           <t>/</t>
         </is>
@@ -4605,15 +3522,15 @@
       <c r="G93" s="5" t="n"/>
     </row>
     <row r="94" ht="18" customHeight="1">
-      <c r="A94" s="14" t="n">
+      <c r="A94" s="10" t="n">
         <v>2022</v>
       </c>
-      <c r="B94" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C94" s="14" t="inlineStr">
+      <c r="B94" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C94" s="10" t="inlineStr">
         <is>
           <t>א</t>
         </is>
@@ -4628,7 +3545,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="F94" s="14" t="inlineStr">
+      <c r="F94" s="10" t="inlineStr">
         <is>
           <t>/</t>
         </is>
@@ -4636,25 +3553,25 @@
       <c r="G94" s="5" t="n"/>
     </row>
     <row r="95" ht="18" customHeight="1">
-      <c r="A95" s="14" t="n">
+      <c r="A95" s="10" t="n">
         <v>2022</v>
       </c>
-      <c r="B95" s="14" t="inlineStr">
-        <is>
-          <t>חורף</t>
-        </is>
-      </c>
-      <c r="C95" s="14" t="inlineStr">
-        <is>
-          <t>ב</t>
-        </is>
-      </c>
-      <c r="D95" s="14" t="inlineStr">
+      <c r="B95" s="10" t="inlineStr">
+        <is>
+          <t>חורף</t>
+        </is>
+      </c>
+      <c r="C95" s="10" t="inlineStr">
+        <is>
+          <t>ב</t>
+        </is>
+      </c>
+      <c r="D95" s="10" t="inlineStr">
         <is>
           <t>חסר</t>
         </is>
       </c>
-      <c r="F95" s="14" t="inlineStr">
+      <c r="F95" s="10" t="inlineStr">
         <is>
           <t>/</t>
         </is>
@@ -4662,9 +3579,10 @@
       <c r="G95" s="5" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B10:C10"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B7:C7"/>
@@ -4674,27 +3592,27 @@
     <mergeCell ref="A2:C2"/>
   </mergeCells>
   <conditionalFormatting sqref="E16:E1000">
-    <cfRule type="expression" priority="7" dxfId="0" stopIfTrue="1">
+    <cfRule type="expression" priority="15" dxfId="0" stopIfTrue="1">
       <formula>ISNUMBER(A16)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:F1048576">
-    <cfRule type="expression" priority="6" dxfId="13" stopIfTrue="1">
+  <conditionalFormatting sqref="A1:F9 A11:F1048576 A10:B10 D10:F10">
+    <cfRule type="expression" priority="6" dxfId="6" stopIfTrue="1">
       <formula>AND(XFD1 = "חסר", B1 = "/")</formula>
     </cfRule>
-    <cfRule type="expression" priority="11" dxfId="5" stopIfTrue="1">
+    <cfRule type="expression" priority="7" dxfId="5" stopIfTrue="1">
       <formula>A1="/"</formula>
     </cfRule>
-    <cfRule type="expression" priority="12" dxfId="4" stopIfTrue="1">
+    <cfRule type="expression" priority="11" dxfId="4" stopIfTrue="1">
       <formula>A1="חסר"</formula>
     </cfRule>
-    <cfRule type="expression" priority="13" dxfId="3" stopIfTrue="1">
+    <cfRule type="expression" priority="12" dxfId="3" stopIfTrue="1">
       <formula>A1="-"</formula>
     </cfRule>
-    <cfRule type="expression" priority="14" dxfId="2" stopIfTrue="1">
+    <cfRule type="expression" priority="13" dxfId="2" stopIfTrue="1">
       <formula>A1="v"</formula>
     </cfRule>
-    <cfRule type="expression" priority="15" dxfId="1" stopIfTrue="1">
+    <cfRule type="expression" priority="14" dxfId="1" stopIfTrue="1">
       <formula>A1="x"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>